<commit_message>
OOP + display la numere
</commit_message>
<xml_diff>
--- a/Algoritmi Fundamentali/Prezenta.xlsx
+++ b/Algoritmi Fundamentali/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2024_2027\Algoritmi Fundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A2DCAA-A740-4FC9-8FAD-95A435BDFB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3DB692-A0E4-4FA0-B541-CC4F8B0F0BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Prenume Nume</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>David Varga</t>
+  </si>
+  <si>
+    <t>Darius Pantea</t>
+  </si>
+  <si>
+    <t>Paul Derecichei</t>
+  </si>
+  <si>
+    <t>Vanesa Marcu</t>
+  </si>
+  <si>
+    <t>Zsolt Dudas</t>
   </si>
 </sst>
 </file>
@@ -383,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -424,30 +436,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Default" xfId="1" xr:uid="{C2A1F133-5CCB-48A4-A954-37FCB6A8888E}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -736,11 +737,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S37"/>
+  <dimension ref="B2:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -815,7 +816,9 @@
       <c r="D3" s="12">
         <v>2</v>
       </c>
-      <c r="E3" s="12"/>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -829,7 +832,7 @@
       <c r="P3" s="13"/>
       <c r="Q3" s="10">
         <f t="shared" ref="Q3:Q30" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R3" s="4"/>
       <c r="S3" s="5"/>
@@ -839,24 +842,26 @@
         <v>45</v>
       </c>
       <c r="C4" s="14"/>
-      <c r="D4" s="19">
-        <v>2</v>
-      </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="7"/>
@@ -868,24 +873,26 @@
       <c r="C5" s="14">
         <v>1</v>
       </c>
-      <c r="D5" s="19">
-        <v>1</v>
-      </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
       <c r="P5" s="15"/>
       <c r="Q5" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R5" s="6"/>
       <c r="S5" s="7"/>
@@ -897,24 +904,26 @@
       <c r="C6" s="14">
         <v>1</v>
       </c>
-      <c r="D6" s="19">
-        <v>1</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
       <c r="P6" s="15"/>
       <c r="Q6" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R6" s="6"/>
       <c r="S6" s="7"/>
@@ -924,24 +933,26 @@
         <v>41</v>
       </c>
       <c r="C7" s="14"/>
-      <c r="D7" s="19">
-        <v>2</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
       <c r="P7" s="15"/>
       <c r="Q7" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R7" s="6"/>
       <c r="S7" s="7"/>
@@ -951,24 +962,26 @@
         <v>35</v>
       </c>
       <c r="C8" s="14"/>
-      <c r="D8" s="19">
-        <v>2</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R8" s="6"/>
       <c r="S8" s="7"/>
@@ -980,24 +993,26 @@
       <c r="C9" s="14">
         <v>1</v>
       </c>
-      <c r="D9" s="19">
-        <v>2</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
       <c r="P9" s="15"/>
       <c r="Q9" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R9" s="6"/>
       <c r="S9" s="7"/>
@@ -1009,20 +1024,20 @@
       <c r="C10" s="14">
         <v>1</v>
       </c>
-      <c r="D10" s="19">
-        <v>2</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
       <c r="P10" s="15"/>
       <c r="Q10" s="10">
         <f t="shared" si="0"/>
@@ -1036,20 +1051,20 @@
         <v>36</v>
       </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="19">
-        <v>1</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
       <c r="P11" s="15"/>
       <c r="Q11" s="10">
         <f t="shared" si="0"/>
@@ -1065,20 +1080,20 @@
       <c r="C12" s="14">
         <v>1</v>
       </c>
-      <c r="D12" s="19">
-        <v>1</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
       <c r="P12" s="15"/>
       <c r="Q12" s="10">
         <f t="shared" si="0"/>
@@ -1094,20 +1109,20 @@
       <c r="C13" s="14">
         <v>1</v>
       </c>
-      <c r="D13" s="19">
-        <v>1</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="10">
         <f t="shared" si="0"/>
@@ -1121,24 +1136,26 @@
         <v>34</v>
       </c>
       <c r="C14" s="14"/>
-      <c r="D14" s="19">
-        <v>2</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
       <c r="P14" s="15"/>
       <c r="Q14" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R14" s="6"/>
       <c r="S14" s="7"/>
@@ -1148,24 +1165,24 @@
         <v>39</v>
       </c>
       <c r="C15" s="14"/>
-      <c r="D15" s="19">
-        <v>1</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
       <c r="P15" s="15"/>
       <c r="Q15" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="7"/>
@@ -1177,24 +1194,26 @@
       <c r="C16" s="14">
         <v>1</v>
       </c>
-      <c r="D16" s="19">
-        <v>1</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
       <c r="P16" s="15"/>
       <c r="Q16" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R16" s="6"/>
       <c r="S16" s="7"/>
@@ -1204,20 +1223,20 @@
         <v>46</v>
       </c>
       <c r="C17" s="14"/>
-      <c r="D17" s="19">
-        <v>2</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
       <c r="P17" s="15"/>
       <c r="Q17" s="16">
         <f t="shared" si="0"/>
@@ -1231,20 +1250,20 @@
         <v>37</v>
       </c>
       <c r="C18" s="14"/>
-      <c r="D18" s="19">
-        <v>1</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
       <c r="P18" s="15"/>
       <c r="Q18" s="10">
         <f t="shared" si="0"/>
@@ -1258,20 +1277,20 @@
         <v>32</v>
       </c>
       <c r="C19" s="14"/>
-      <c r="D19" s="19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
       <c r="P19" s="15"/>
       <c r="Q19" s="10">
         <f t="shared" si="0"/>
@@ -1287,20 +1306,20 @@
       <c r="C20" s="14">
         <v>1</v>
       </c>
-      <c r="D20" s="19">
-        <v>1</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
       <c r="P20" s="15"/>
       <c r="Q20" s="10">
         <f t="shared" si="0"/>
@@ -1316,24 +1335,26 @@
       <c r="C21" s="14">
         <v>1</v>
       </c>
-      <c r="D21" s="19">
-        <v>2</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
+      <c r="D21" s="2">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
       <c r="P21" s="15"/>
       <c r="Q21" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R21" s="6"/>
       <c r="S21" s="7"/>
@@ -1343,24 +1364,26 @@
         <v>44</v>
       </c>
       <c r="C22" s="14"/>
-      <c r="D22" s="19">
-        <v>1</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
       <c r="P22" s="15"/>
       <c r="Q22" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R22" s="6"/>
       <c r="S22" s="7"/>
@@ -1370,20 +1393,20 @@
         <v>38</v>
       </c>
       <c r="C23" s="14"/>
-      <c r="D23" s="19">
-        <v>1</v>
-      </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
       <c r="P23" s="15"/>
       <c r="Q23" s="10">
         <f t="shared" si="0"/>
@@ -1397,20 +1420,20 @@
         <v>47</v>
       </c>
       <c r="C24" s="14"/>
-      <c r="D24" s="19">
-        <v>2</v>
-      </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
+      <c r="D24" s="2">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="10">
         <f t="shared" si="0"/>
@@ -1424,20 +1447,20 @@
         <v>43</v>
       </c>
       <c r="C25" s="14"/>
-      <c r="D25" s="19">
-        <v>1</v>
-      </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="10">
         <f t="shared" si="0"/>
@@ -1453,24 +1476,26 @@
       <c r="C26" s="14">
         <v>1</v>
       </c>
-      <c r="D26" s="19">
-        <v>2</v>
-      </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
+      <c r="D26" s="2">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
       <c r="P26" s="15"/>
       <c r="Q26" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R26" s="6"/>
       <c r="S26" s="7"/>
@@ -1480,24 +1505,26 @@
         <v>40</v>
       </c>
       <c r="C27" s="14"/>
-      <c r="D27" s="19">
-        <v>2</v>
-      </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
+      <c r="D27" s="2">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
       <c r="P27" s="15"/>
       <c r="Q27" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R27" s="6"/>
       <c r="S27" s="7"/>
@@ -1509,24 +1536,26 @@
       <c r="C28" s="14">
         <v>1</v>
       </c>
-      <c r="D28" s="19">
-        <v>2</v>
-      </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
+      <c r="D28" s="2">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R28" s="6"/>
       <c r="S28" s="7"/>
@@ -1536,24 +1565,26 @@
         <v>42</v>
       </c>
       <c r="C29" s="14"/>
-      <c r="D29" s="19">
-        <v>1</v>
-      </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
       <c r="P29" s="15"/>
       <c r="Q29" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R29" s="6"/>
       <c r="S29" s="7"/>
@@ -1565,18 +1596,18 @@
       <c r="C30" s="14">
         <v>1</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
       <c r="P30" s="15"/>
       <c r="Q30" s="10">
         <f t="shared" si="0"/>
@@ -1592,24 +1623,26 @@
       <c r="C31" s="14">
         <v>1</v>
       </c>
-      <c r="D31" s="19">
-        <v>2</v>
-      </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
+      <c r="D31" s="2">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
       <c r="P31" s="15"/>
       <c r="Q31" s="10">
         <f t="shared" ref="Q31:Q37" si="1">C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R31" s="6"/>
       <c r="S31" s="7"/>
@@ -1621,18 +1654,18 @@
       <c r="C32" s="14">
         <v>1</v>
       </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
       <c r="P32" s="15"/>
       <c r="Q32" s="10">
         <f t="shared" si="1"/>
@@ -1646,24 +1679,16 @@
         <v>48</v>
       </c>
       <c r="C33" s="6"/>
-      <c r="D33" s="18">
-        <v>1</v>
-      </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
       <c r="P33" s="7"/>
       <c r="Q33" s="10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R33" s="6"/>
       <c r="S33" s="7"/>
@@ -1673,20 +1698,9 @@
         <v>49</v>
       </c>
       <c r="C34" s="6"/>
-      <c r="D34" s="18">
-        <v>1</v>
-      </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
       <c r="P34" s="7"/>
       <c r="Q34" s="10">
         <f t="shared" si="1"/>
@@ -1700,20 +1714,9 @@
         <v>50</v>
       </c>
       <c r="C35" s="6"/>
-      <c r="D35" s="18">
-        <v>1</v>
-      </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
       <c r="P35" s="7"/>
       <c r="Q35" s="10">
         <f t="shared" si="1"/>
@@ -1727,20 +1730,9 @@
         <v>51</v>
       </c>
       <c r="C36" s="6"/>
-      <c r="D36" s="18">
-        <v>1</v>
-      </c>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
       <c r="P36" s="7"/>
       <c r="Q36" s="10">
         <f t="shared" si="1"/>
@@ -1754,20 +1746,20 @@
         <v>52</v>
       </c>
       <c r="C37" s="8"/>
-      <c r="D37" s="21">
-        <v>1</v>
-      </c>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
+      <c r="D37" s="18">
+        <v>1</v>
+      </c>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
       <c r="P37" s="9"/>
       <c r="Q37" s="10">
         <f t="shared" si="1"/>
@@ -1775,13 +1767,45 @@
       </c>
       <c r="R37" s="8"/>
       <c r="S37" s="9"/>
+    </row>
+    <row r="38" spans="2:19">
+      <c r="B38" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19">
+      <c r="B39" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19">
+      <c r="B40" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19">
+      <c r="B41" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S32">
     <sortCondition ref="B32"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q37">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
final 2048 + baa filtrelor de imagini + teme de laborator
</commit_message>
<xml_diff>
--- a/Algoritmi Fundamentali/Prezenta.xlsx
+++ b/Algoritmi Fundamentali/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2024_2027\Algoritmi Fundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423FC42A-44D4-4988-A302-095E0274D183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C905657-2115-43D8-B677-78255CF4F25C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Prenume Nume</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Adrian Stefan Basceanu</t>
   </si>
   <si>
-    <t>Aleandru Gabriel Bene</t>
-  </si>
-  <si>
     <t>Darius Florian Ciora</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>Yeremchuk Liudmyla</t>
   </si>
   <si>
-    <t>Mario Aleandru Hutu</t>
-  </si>
-  <si>
     <t>Adelin Sandor</t>
   </si>
   <si>
@@ -202,6 +196,21 @@
   </si>
   <si>
     <t>Casian Stirbe</t>
+  </si>
+  <si>
+    <t>Alexandru Gabriel Bene</t>
+  </si>
+  <si>
+    <t>Mario Alexandru Hutu</t>
+  </si>
+  <si>
+    <t>Iulian Cioara</t>
+  </si>
+  <si>
+    <t>Nora Boros</t>
+  </si>
+  <si>
+    <t>Alina Schmidt</t>
   </si>
 </sst>
 </file>
@@ -401,7 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -434,9 +443,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -745,11 +751,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S43"/>
+  <dimension ref="B2:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -819,7 +825,7 @@
     </row>
     <row r="3" spans="2:19">
       <c r="B3" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6">
@@ -828,7 +834,9 @@
       <c r="E3" s="6">
         <v>1</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -840,15 +848,15 @@
       <c r="O3" s="6"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="8">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>3</v>
+        <f t="shared" ref="Q3:Q43" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>4</v>
       </c>
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="3">
@@ -857,10 +865,13 @@
       <c r="E4" s="3">
         <v>2</v>
       </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="11">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R4" s="9"/>
       <c r="S4" s="10"/>
@@ -880,7 +891,7 @@
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="8">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R5" s="9"/>
@@ -888,7 +899,7 @@
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="C6" s="9">
         <v>1</v>
@@ -901,7 +912,7 @@
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R6" s="9"/>
@@ -909,7 +920,7 @@
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="3">
@@ -920,7 +931,7 @@
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R7" s="9"/>
@@ -928,7 +939,7 @@
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="3">
@@ -939,7 +950,7 @@
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R8" s="9"/>
@@ -947,7 +958,7 @@
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="3">
@@ -958,7 +969,7 @@
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R9" s="9"/>
@@ -977,17 +988,20 @@
       <c r="E10" s="3">
         <v>1</v>
       </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R10" s="9"/>
       <c r="S10" s="10"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
@@ -996,46 +1010,41 @@
         <v>2</v>
       </c>
       <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="8">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R11" s="9"/>
       <c r="S11" s="10"/>
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R12" s="9"/>
       <c r="S12" s="10"/>
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="3">
@@ -1043,7 +1052,7 @@
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R13" s="9"/>
@@ -1051,7 +1060,7 @@
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
@@ -1064,7 +1073,7 @@
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R14" s="9"/>
@@ -1072,7 +1081,7 @@
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
@@ -1085,7 +1094,7 @@
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="8">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R15" s="9"/>
@@ -1093,26 +1102,15 @@
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12">
-        <v>2</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="8">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R16" s="9"/>
@@ -1120,7 +1118,7 @@
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="3">
@@ -1131,7 +1129,7 @@
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R17" s="9"/>
@@ -1139,34 +1137,26 @@
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="9"/>
-      <c r="D18" s="12">
-        <v>1</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R18" s="9"/>
       <c r="S18" s="10"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="3">
@@ -1177,7 +1167,7 @@
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R19" s="9"/>
@@ -1185,7 +1175,7 @@
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="9">
         <v>1</v>
@@ -1194,19 +1184,22 @@
         <v>1</v>
       </c>
       <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
         <v>1</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="R20" s="9"/>
       <c r="S20" s="10"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="3">
@@ -1217,7 +1210,7 @@
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="11">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R21" s="9"/>
@@ -1225,7 +1218,7 @@
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="3">
@@ -1233,7 +1226,7 @@
       </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="8">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R22" s="9"/>
@@ -1241,26 +1234,15 @@
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12">
-        <v>1</v>
-      </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
       <c r="P23" s="10"/>
       <c r="Q23" s="8">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R23" s="9"/>
@@ -1268,23 +1250,26 @@
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="4" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="3">
         <v>1</v>
       </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="8">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="10"/>
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="9">
         <v>1</v>
@@ -1297,7 +1282,7 @@
       </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="8">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R25" s="9"/>
@@ -1316,17 +1301,20 @@
       <c r="E26" s="3">
         <v>1</v>
       </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
       <c r="P26" s="10"/>
       <c r="Q26" s="8">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R26" s="9"/>
       <c r="S26" s="10"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="3">
@@ -1335,17 +1323,20 @@
       <c r="E27" s="3">
         <v>2</v>
       </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
       <c r="P27" s="10"/>
       <c r="Q27" s="8">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="R27" s="9"/>
       <c r="S27" s="10"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="3">
@@ -1353,7 +1344,7 @@
       </c>
       <c r="P28" s="10"/>
       <c r="Q28" s="8">
-        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R28" s="9"/>
@@ -1361,34 +1352,26 @@
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C29" s="9"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12">
-        <v>2</v>
-      </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
+      <c r="E29" s="3">
+        <v>2</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
       <c r="P29" s="10"/>
       <c r="Q29" s="8">
-        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="10"/>
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="3">
@@ -1396,7 +1379,7 @@
       </c>
       <c r="P30" s="10"/>
       <c r="Q30" s="8">
-        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R30" s="9"/>
@@ -1404,7 +1387,7 @@
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="3">
@@ -1412,7 +1395,7 @@
       </c>
       <c r="P31" s="10"/>
       <c r="Q31" s="8">
-        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R31" s="9"/>
@@ -1420,7 +1403,7 @@
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="9">
         <v>1</v>
@@ -1429,19 +1412,22 @@
         <v>2</v>
       </c>
       <c r="E32" s="3">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3">
         <v>1</v>
       </c>
       <c r="P32" s="10"/>
       <c r="Q32" s="8">
-        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R32" s="9"/>
       <c r="S32" s="10"/>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="3">
@@ -1452,7 +1438,7 @@
       </c>
       <c r="P33" s="10"/>
       <c r="Q33" s="8">
-        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R33" s="9"/>
@@ -1460,7 +1446,7 @@
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="9">
         <v>1</v>
@@ -1470,18 +1456,21 @@
       </c>
       <c r="E34" s="3">
         <v>2</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1</v>
       </c>
       <c r="P34" s="10"/>
       <c r="Q34" s="8">
-        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="R34" s="9"/>
       <c r="S34" s="10"/>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="3">
@@ -1492,7 +1481,7 @@
       </c>
       <c r="P35" s="10"/>
       <c r="Q35" s="8">
-        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R35" s="9"/>
@@ -1507,7 +1496,7 @@
       </c>
       <c r="P36" s="10"/>
       <c r="Q36" s="8">
-        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R36" s="9"/>
@@ -1526,17 +1515,20 @@
       <c r="E37" s="3">
         <v>1</v>
       </c>
+      <c r="F37" s="3">
+        <v>1</v>
+      </c>
       <c r="P37" s="10"/>
       <c r="Q37" s="8">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R37" s="9"/>
       <c r="S37" s="10"/>
     </row>
     <row r="38" spans="2:19">
-      <c r="B38" s="13" t="s">
-        <v>51</v>
+      <c r="B38" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="3">
@@ -1545,44 +1537,36 @@
       <c r="E38" s="3">
         <v>1</v>
       </c>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
       <c r="P38" s="10"/>
       <c r="Q38" s="8">
-        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R38" s="9"/>
       <c r="S38" s="10"/>
     </row>
     <row r="39" spans="2:19">
-      <c r="B39" s="13" t="s">
-        <v>55</v>
+      <c r="B39" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="C39" s="9"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12">
-        <v>1</v>
-      </c>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
-      <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
-      <c r="O39" s="12"/>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
       <c r="P39" s="10"/>
       <c r="Q39" s="8">
-        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R39" s="9"/>
       <c r="S39" s="10"/>
     </row>
     <row r="40" spans="2:19">
-      <c r="B40" s="13" t="s">
-        <v>49</v>
+      <c r="B40" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="3">
@@ -1593,15 +1577,15 @@
       </c>
       <c r="P40" s="10"/>
       <c r="Q40" s="8">
-        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R40" s="9"/>
       <c r="S40" s="10"/>
     </row>
     <row r="41" spans="2:19">
-      <c r="B41" s="13" t="s">
-        <v>48</v>
+      <c r="B41" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="3">
@@ -1610,55 +1594,85 @@
       <c r="E41" s="3">
         <v>1</v>
       </c>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
       <c r="P41" s="10"/>
       <c r="Q41" s="8">
-        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R41" s="9"/>
       <c r="S41" s="10"/>
     </row>
     <row r="42" spans="2:19">
-      <c r="B42" s="13" t="s">
-        <v>31</v>
+      <c r="B42" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="C42" s="9">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3">
         <v>1</v>
       </c>
       <c r="P42" s="10"/>
       <c r="Q42" s="8">
-        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R42" s="9"/>
       <c r="S42" s="10"/>
     </row>
     <row r="43" spans="2:19">
-      <c r="B43" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15">
-        <v>1</v>
-      </c>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="16"/>
+      <c r="B43" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14">
+        <v>1</v>
+      </c>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="15"/>
       <c r="Q43" s="8">
-        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
-        <v>1</v>
-      </c>
-      <c r="R43" s="14"/>
-      <c r="S43" s="16"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R43" s="13"/>
+      <c r="S43" s="15"/>
+    </row>
+    <row r="44" spans="2:19">
+      <c r="B44" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:19">
+      <c r="B45" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:19">
+      <c r="B46" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S43">

</xml_diff>

<commit_message>
am facut 4 filtre pe imagine
</commit_message>
<xml_diff>
--- a/Algoritmi Fundamentali/Prezenta.xlsx
+++ b/Algoritmi Fundamentali/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2024_2027\Algoritmi Fundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C905657-2115-43D8-B677-78255CF4F25C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB3B2A9-30B4-4BAD-9FD2-305C09FA9423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,7 +210,7 @@
     <t>Nora Boros</t>
   </si>
   <si>
-    <t>Alina Schmidt</t>
+    <t>Anita Schmidt</t>
   </si>
 </sst>
 </file>
@@ -754,8 +754,8 @@
   <dimension ref="B2:S46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H46" sqref="H46"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -866,12 +866,12 @@
         <v>2</v>
       </c>
       <c r="F4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R4" s="9"/>
       <c r="S4" s="10"/>
@@ -889,10 +889,13 @@
       <c r="E5" s="3">
         <v>1</v>
       </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="10"/>
@@ -910,10 +913,13 @@
       <c r="E6" s="3">
         <v>1</v>
       </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R6" s="9"/>
       <c r="S6" s="10"/>
@@ -929,10 +935,13 @@
       <c r="E7" s="3">
         <v>2</v>
       </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R7" s="9"/>
       <c r="S7" s="10"/>
@@ -948,10 +957,13 @@
       <c r="E8" s="3">
         <v>1</v>
       </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R8" s="9"/>
       <c r="S8" s="10"/>
@@ -1013,12 +1025,12 @@
         <v>1</v>
       </c>
       <c r="F11" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R11" s="9"/>
       <c r="S11" s="10"/>
@@ -1032,12 +1044,12 @@
         <v>1</v>
       </c>
       <c r="F12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R12" s="9"/>
       <c r="S12" s="10"/>
@@ -1050,10 +1062,13 @@
       <c r="D13" s="3">
         <v>1</v>
       </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13" s="9"/>
       <c r="S13" s="10"/>
@@ -1127,10 +1142,13 @@
       <c r="E17" s="3">
         <v>2</v>
       </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R17" s="9"/>
       <c r="S17" s="10"/>
@@ -1165,10 +1183,13 @@
       <c r="E19" s="3">
         <v>1</v>
       </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R19" s="9"/>
       <c r="S19" s="10"/>
@@ -1187,12 +1208,12 @@
         <v>1</v>
       </c>
       <c r="F20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R20" s="9"/>
       <c r="S20" s="10"/>
@@ -1257,12 +1278,12 @@
         <v>1</v>
       </c>
       <c r="F24" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="10"/>
@@ -1280,10 +1301,13 @@
       <c r="E25" s="3">
         <v>1</v>
       </c>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R25" s="9"/>
       <c r="S25" s="10"/>
@@ -1359,12 +1383,12 @@
         <v>2</v>
       </c>
       <c r="F29" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P29" s="10"/>
       <c r="Q29" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="10"/>
@@ -1436,10 +1460,13 @@
       <c r="E33" s="3">
         <v>2</v>
       </c>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
       <c r="P33" s="10"/>
       <c r="Q33" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R33" s="9"/>
       <c r="S33" s="10"/>
@@ -1458,12 +1485,12 @@
         <v>2</v>
       </c>
       <c r="F34" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P34" s="10"/>
       <c r="Q34" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R34" s="9"/>
       <c r="S34" s="10"/>
@@ -1479,10 +1506,13 @@
       <c r="E35" s="3">
         <v>1</v>
       </c>
+      <c r="F35" s="3">
+        <v>1</v>
+      </c>
       <c r="P35" s="10"/>
       <c r="Q35" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R35" s="9"/>
       <c r="S35" s="10"/>
@@ -1516,12 +1546,12 @@
         <v>1</v>
       </c>
       <c r="F37" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P37" s="10"/>
       <c r="Q37" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R37" s="9"/>
       <c r="S37" s="10"/>
@@ -1538,12 +1568,12 @@
         <v>1</v>
       </c>
       <c r="F38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P38" s="10"/>
       <c r="Q38" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R38" s="9"/>
       <c r="S38" s="10"/>
@@ -1671,7 +1701,7 @@
         <v>61</v>
       </c>
       <c r="F46" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inceput RPG + baza matrici vizual
</commit_message>
<xml_diff>
--- a/Algoritmi Fundamentali/Prezenta.xlsx
+++ b/Algoritmi Fundamentali/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2024_2027\Algoritmi Fundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB3B2A9-30B4-4BAD-9FD2-305C09FA9423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8FCEDD-35A5-4B2D-B808-4DE782F69608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Prenume Nume</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>Anita Schmidt</t>
+  </si>
+  <si>
+    <t>Emil Macarie</t>
+  </si>
+  <si>
+    <t>Laurentiu Flonta</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -455,6 +461,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -751,11 +763,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S46"/>
+  <dimension ref="B2:S48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -837,7 +849,9 @@
       <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -848,8 +862,8 @@
       <c r="O3" s="6"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="8">
-        <f t="shared" ref="Q3:Q43" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>4</v>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>5</v>
       </c>
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
@@ -868,10 +882,13 @@
       <c r="F4" s="3">
         <v>2</v>
       </c>
+      <c r="G4" s="3">
+        <v>2</v>
+      </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="11">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
+        <v>8</v>
       </c>
       <c r="R4" s="9"/>
       <c r="S4" s="10"/>
@@ -892,55 +909,64 @@
       <c r="F5" s="3">
         <v>1</v>
       </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <v>5</v>
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="10"/>
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C6" s="9"/>
       <c r="D6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
         <v>1</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <v>6</v>
       </c>
       <c r="R6" s="9"/>
       <c r="S6" s="10"/>
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="9"/>
+        <v>57</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
       <c r="D7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
         <v>1</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
-        <f t="shared" si="0"/>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
         <v>5</v>
       </c>
       <c r="R7" s="9"/>
@@ -960,10 +986,13 @@
       <c r="F8" s="3">
         <v>1</v>
       </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <v>4</v>
       </c>
       <c r="R8" s="9"/>
       <c r="S8" s="10"/>
@@ -981,7 +1010,7 @@
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8">
-        <f t="shared" si="0"/>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
         <v>3</v>
       </c>
       <c r="R9" s="9"/>
@@ -989,31 +1018,26 @@
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="9">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C10" s="9"/>
       <c r="F10" s="3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <v>4</v>
       </c>
       <c r="R10" s="9"/>
       <c r="S10" s="10"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
@@ -1025,11 +1049,14 @@
         <v>1</v>
       </c>
       <c r="F11" s="3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="8">
-        <f t="shared" si="0"/>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
         <v>6</v>
       </c>
       <c r="R11" s="9"/>
@@ -1037,58 +1064,70 @@
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
       <c r="E12" s="3">
         <v>1</v>
       </c>
       <c r="F12" s="3">
         <v>2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <v>7</v>
       </c>
       <c r="R12" s="9"/>
       <c r="S12" s="10"/>
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C13" s="9"/>
-      <c r="D13" s="3">
+      <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <v>5</v>
       </c>
       <c r="R13" s="9"/>
       <c r="S13" s="10"/>
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="9">
-        <v>1</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C14" s="9"/>
       <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
         <v>1</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8">
-        <f t="shared" si="0"/>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
         <v>3</v>
       </c>
       <c r="R14" s="9"/>
@@ -1096,7 +1135,7 @@
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
@@ -1109,7 +1148,7 @@
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="8">
-        <f t="shared" si="0"/>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
         <v>3</v>
       </c>
       <c r="R15" s="9"/>
@@ -1117,70 +1156,78 @@
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
       <c r="E16" s="3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
       </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <v>4</v>
       </c>
       <c r="R16" s="9"/>
       <c r="S16" s="10"/>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="4" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="3">
-        <v>2</v>
-      </c>
       <c r="E17" s="3">
         <v>2</v>
       </c>
-      <c r="F17" s="3">
-        <v>1</v>
+      <c r="G17" s="3">
+        <v>2</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <v>4</v>
       </c>
       <c r="R17" s="9"/>
       <c r="S17" s="10"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="4" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <v>7</v>
       </c>
       <c r="R18" s="9"/>
       <c r="S18" s="10"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="4" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="3">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3">
         <v>1</v>
       </c>
       <c r="F19" s="3">
@@ -1188,299 +1235,286 @@
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <v>2</v>
       </c>
       <c r="R19" s="9"/>
       <c r="S19" s="10"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="9">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C20" s="9"/>
       <c r="D20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
       </c>
       <c r="F20" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <v>4</v>
       </c>
       <c r="R20" s="9"/>
       <c r="S20" s="10"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
       <c r="D21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
       </c>
+      <c r="F21" s="3">
+        <v>2</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
       <c r="P21" s="10"/>
-      <c r="Q21" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+      <c r="Q21" s="8">
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <v>6</v>
       </c>
       <c r="R21" s="9"/>
       <c r="S21" s="10"/>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="C22" s="9"/>
-      <c r="D22" s="3">
-        <v>1</v>
+      <c r="G22" s="3">
+        <v>2</v>
       </c>
       <c r="P22" s="10"/>
-      <c r="Q22" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="Q22" s="11"/>
       <c r="R22" s="9"/>
       <c r="S22" s="10"/>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="4" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C23" s="9"/>
+      <c r="D23" s="3">
+        <v>2</v>
+      </c>
       <c r="E23" s="3">
         <v>1</v>
       </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
       <c r="P23" s="10"/>
-      <c r="Q23" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="Q23" s="11">
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <v>4</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="10"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C24" s="9"/>
-      <c r="D24" s="3">
-        <v>1</v>
-      </c>
       <c r="F24" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P24" s="10"/>
-      <c r="Q24" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
+      <c r="Q24" s="11"/>
       <c r="R24" s="9"/>
       <c r="S24" s="10"/>
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="9">
-        <v>1</v>
-      </c>
-      <c r="D25" s="3">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3">
-        <v>1</v>
-      </c>
-      <c r="F25" s="3">
+        <v>63</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="G25" s="3">
         <v>1</v>
       </c>
       <c r="P25" s="10"/>
-      <c r="Q25" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
+      <c r="Q25" s="11"/>
       <c r="R25" s="9"/>
       <c r="S25" s="10"/>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="9">
-        <v>1</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C26" s="9"/>
       <c r="D26" s="3">
-        <v>2</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-      <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="P26" s="10"/>
       <c r="Q26" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <v>1</v>
       </c>
       <c r="R26" s="9"/>
       <c r="S26" s="10"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="4" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C27" s="9"/>
-      <c r="D27" s="3">
-        <v>1</v>
-      </c>
       <c r="E27" s="3">
-        <v>2</v>
-      </c>
-      <c r="F27" s="3">
         <v>1</v>
       </c>
       <c r="P27" s="10"/>
       <c r="Q27" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <v>1</v>
       </c>
       <c r="R27" s="9"/>
       <c r="S27" s="10"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="4" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="3">
         <v>1</v>
       </c>
+      <c r="F28" s="3">
+        <v>2</v>
+      </c>
+      <c r="G28" s="3">
+        <v>2</v>
+      </c>
       <c r="P28" s="10"/>
       <c r="Q28" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <v>5</v>
       </c>
       <c r="R28" s="9"/>
       <c r="S28" s="10"/>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
       <c r="E29" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" s="3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1</v>
       </c>
       <c r="P29" s="10"/>
       <c r="Q29" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>5</v>
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="10"/>
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
       <c r="D30" s="3">
         <v>2</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3">
+        <v>1</v>
       </c>
       <c r="P30" s="10"/>
       <c r="Q30" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>6</v>
       </c>
       <c r="R30" s="9"/>
       <c r="S30" s="10"/>
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="4" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="C31" s="9"/>
-      <c r="D31" s="3">
+      <c r="F31" s="3">
         <v>1</v>
       </c>
       <c r="P31" s="10"/>
-      <c r="Q31" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="Q31" s="11"/>
       <c r="R31" s="9"/>
       <c r="S31" s="10"/>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="9">
-        <v>1</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C32" s="9"/>
       <c r="D32" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
       </c>
       <c r="P32" s="10"/>
       <c r="Q32" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <v>4</v>
       </c>
       <c r="R32" s="9"/>
       <c r="S32" s="10"/>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="3">
-        <v>2</v>
-      </c>
-      <c r="E33" s="3">
-        <v>2</v>
-      </c>
-      <c r="F33" s="3">
         <v>1</v>
       </c>
       <c r="P33" s="10"/>
       <c r="Q33" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <v>1</v>
       </c>
       <c r="R33" s="9"/>
       <c r="S33" s="10"/>
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="9">
-        <v>1</v>
-      </c>
-      <c r="D34" s="3">
-        <v>2</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C34" s="9"/>
       <c r="E34" s="3">
         <v>2</v>
       </c>
@@ -1489,44 +1523,39 @@
       </c>
       <c r="P34" s="10"/>
       <c r="Q34" s="8">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <v>4</v>
       </c>
       <c r="R34" s="9"/>
       <c r="S34" s="10"/>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="3">
-        <v>1</v>
-      </c>
-      <c r="E35" s="3">
-        <v>1</v>
-      </c>
-      <c r="F35" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P35" s="10"/>
       <c r="Q35" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <v>2</v>
       </c>
       <c r="R35" s="9"/>
       <c r="S35" s="10"/>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="9">
+        <v>41</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="3">
         <v>1</v>
       </c>
       <c r="P36" s="10"/>
       <c r="Q36" s="8">
-        <f t="shared" si="0"/>
+        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
         <v>1</v>
       </c>
       <c r="R36" s="9"/>
@@ -1534,7 +1563,7 @@
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C37" s="9">
         <v>1</v>
@@ -1546,11 +1575,14 @@
         <v>1</v>
       </c>
       <c r="F37" s="3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1</v>
       </c>
       <c r="P37" s="10"/>
       <c r="Q37" s="8">
-        <f t="shared" si="0"/>
+        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
         <v>6</v>
       </c>
       <c r="R37" s="9"/>
@@ -1558,45 +1590,56 @@
     </row>
     <row r="38" spans="2:19">
       <c r="B38" s="12" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F38" s="3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1</v>
       </c>
       <c r="P38" s="10"/>
       <c r="Q38" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <v>6</v>
       </c>
       <c r="R38" s="9"/>
       <c r="S38" s="10"/>
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="C39" s="9">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3">
+        <v>2</v>
+      </c>
       <c r="E39" s="3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F39" s="3">
+        <v>2</v>
       </c>
       <c r="P39" s="10"/>
       <c r="Q39" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <v>7</v>
       </c>
       <c r="R39" s="9"/>
       <c r="S39" s="10"/>
     </row>
     <row r="40" spans="2:19">
       <c r="B40" s="12" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="3">
@@ -1605,65 +1648,76 @@
       <c r="E40" s="3">
         <v>1</v>
       </c>
+      <c r="F40" s="3">
+        <v>1</v>
+      </c>
       <c r="P40" s="10"/>
       <c r="Q40" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
+        <v>3</v>
       </c>
       <c r="R40" s="9"/>
       <c r="S40" s="10"/>
     </row>
     <row r="41" spans="2:19">
       <c r="B41" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="3">
-        <v>1</v>
-      </c>
-      <c r="E41" s="3">
-        <v>1</v>
-      </c>
-      <c r="F41" s="3">
+        <v>21</v>
+      </c>
+      <c r="C41" s="9">
         <v>1</v>
       </c>
       <c r="P41" s="10"/>
       <c r="Q41" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <v>1</v>
       </c>
       <c r="R41" s="9"/>
       <c r="S41" s="10"/>
     </row>
     <row r="42" spans="2:19">
       <c r="B42" s="12" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C42" s="9">
         <v>1</v>
       </c>
+      <c r="D42" s="3">
+        <v>2</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
       <c r="F42" s="3">
+        <v>2</v>
+      </c>
+      <c r="G42" s="3">
         <v>1</v>
       </c>
       <c r="P42" s="10"/>
       <c r="Q42" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
+        <v>7</v>
       </c>
       <c r="R42" s="9"/>
       <c r="S42" s="10"/>
     </row>
     <row r="43" spans="2:19">
       <c r="B43" s="12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C43" s="13"/>
-      <c r="D43" s="14"/>
+      <c r="D43" s="14">
+        <v>1</v>
+      </c>
       <c r="E43" s="14">
         <v>1</v>
       </c>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
+      <c r="F43" s="14">
+        <v>2</v>
+      </c>
+      <c r="G43" s="14">
+        <v>1</v>
+      </c>
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
@@ -1674,41 +1728,139 @@
       <c r="O43" s="14"/>
       <c r="P43" s="15"/>
       <c r="Q43" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
+        <v>5</v>
       </c>
       <c r="R43" s="13"/>
       <c r="S43" s="15"/>
     </row>
     <row r="44" spans="2:19">
       <c r="B44" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F44" s="3">
-        <v>1</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16">
+        <v>1</v>
+      </c>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+      <c r="Q44" s="8">
+        <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
+        <v>1</v>
+      </c>
+      <c r="R44" s="16"/>
+      <c r="S44" s="16"/>
     </row>
     <row r="45" spans="2:19">
       <c r="B45" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F45" s="3">
-        <v>1</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C45" s="16"/>
+      <c r="D45" s="3">
+        <v>1</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3">
+        <v>1</v>
+      </c>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="8">
+        <f>C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
+        <v>3</v>
+      </c>
+      <c r="R45" s="16"/>
+      <c r="S45" s="16"/>
     </row>
     <row r="46" spans="2:19">
       <c r="B46" s="12" t="s">
-        <v>61</v>
+        <v>46</v>
+      </c>
+      <c r="C46" s="16"/>
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
       </c>
       <c r="F46" s="3">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G46" s="3">
+        <v>1</v>
+      </c>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="8">
+        <f>C46+D46+E46+F46+G46+H46+I46+J46+K46+L46+M46+N46+O46+P46</f>
+        <v>4</v>
+      </c>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+    </row>
+    <row r="47" spans="2:19">
+      <c r="B47" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="16">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3">
+        <v>1</v>
+      </c>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="8">
+        <f>C47+D47+E47+F47+G47+H47+I47+J47+K47+L47+M47+N47+O47+P47</f>
+        <v>3</v>
+      </c>
+      <c r="R47" s="16"/>
+      <c r="S47" s="16"/>
+    </row>
+    <row r="48" spans="2:19">
+      <c r="B48" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16">
+        <v>1</v>
+      </c>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="16"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+      <c r="Q48" s="17">
+        <f>C48+D48+E48+F48+G48+H48+I48+J48+K48+L48+M48+N48+O48+P48</f>
+        <v>1</v>
+      </c>
+      <c r="R48" s="16"/>
+      <c r="S48" s="16"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S43">
-    <sortCondition ref="B43"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S48">
+    <sortCondition ref="B48"/>
   </sortState>
-  <conditionalFormatting sqref="Q3:Q43">
+  <conditionalFormatting sqref="Q3:Q47">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>14</formula>
     </cfRule>

</xml_diff>

<commit_message>
algoritmul lui lee pentru gasirea path-ului
</commit_message>
<xml_diff>
--- a/Algoritmi Fundamentali/Prezenta.xlsx
+++ b/Algoritmi Fundamentali/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2024_2027\Algoritmi Fundamentali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06406DDD-3ABB-416B-92B2-6B8B7C70B007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026C46B9-F55D-42C6-B3F9-69CD41B38D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -770,7 +770,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -897,12 +897,12 @@
         <v>1</v>
       </c>
       <c r="L4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="8">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R4" s="9"/>
       <c r="S4" s="10"/>
@@ -936,12 +936,12 @@
         <v>2</v>
       </c>
       <c r="L5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="8">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="10"/>
@@ -991,10 +991,13 @@
       <c r="K7" s="3">
         <v>1</v>
       </c>
+      <c r="L7" s="3">
+        <v>1</v>
+      </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R7" s="9"/>
       <c r="S7" s="10"/>
@@ -1025,12 +1028,12 @@
         <v>2</v>
       </c>
       <c r="L8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R8" s="9"/>
       <c r="S8" s="10"/>
@@ -1055,10 +1058,13 @@
       <c r="H9" s="3">
         <v>1</v>
       </c>
+      <c r="L9" s="3">
+        <v>1</v>
+      </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R9" s="9"/>
       <c r="S9" s="10"/>
@@ -1094,12 +1100,12 @@
         <v>2</v>
       </c>
       <c r="L11" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R11" s="9"/>
       <c r="S11" s="10"/>
@@ -1166,12 +1172,12 @@
         <v>1</v>
       </c>
       <c r="L13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R13" s="9"/>
       <c r="S13" s="10"/>
@@ -1303,10 +1309,13 @@
       <c r="K18" s="3">
         <v>2</v>
       </c>
+      <c r="L18" s="3">
+        <v>2</v>
+      </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="R18" s="9"/>
       <c r="S18" s="10"/>
@@ -1335,12 +1344,12 @@
         <v>2</v>
       </c>
       <c r="L19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R19" s="9"/>
       <c r="S19" s="10"/>
@@ -1357,12 +1366,12 @@
         <v>1</v>
       </c>
       <c r="L20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R20" s="9"/>
       <c r="S20" s="10"/>
@@ -1439,10 +1448,13 @@
       <c r="J23" s="3">
         <v>2</v>
       </c>
+      <c r="L23" s="3">
+        <v>1</v>
+      </c>
       <c r="P23" s="10"/>
       <c r="Q23" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="10"/>
@@ -1455,10 +1467,13 @@
       <c r="I24" s="3">
         <v>1</v>
       </c>
+      <c r="L24" s="3">
+        <v>1</v>
+      </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="10"/>
@@ -1472,12 +1487,12 @@
         <v>2</v>
       </c>
       <c r="L25" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R25" s="9"/>
       <c r="S25" s="10"/>
@@ -1502,10 +1517,13 @@
       <c r="I26" s="3">
         <v>2</v>
       </c>
+      <c r="L26" s="3">
+        <v>1</v>
+      </c>
       <c r="P26" s="10"/>
       <c r="Q26" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R26" s="9"/>
       <c r="S26" s="10"/>
@@ -1689,12 +1707,12 @@
         <v>2</v>
       </c>
       <c r="L34" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P34" s="10"/>
       <c r="Q34" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R34" s="9"/>
       <c r="S34" s="10"/>
@@ -1764,12 +1782,12 @@
         <v>2</v>
       </c>
       <c r="L37" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P37" s="10"/>
       <c r="Q37" s="8">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R37" s="9"/>
       <c r="S37" s="10"/>
@@ -1880,10 +1898,13 @@
       <c r="K41" s="3">
         <v>1</v>
       </c>
+      <c r="L41" s="3">
+        <v>1</v>
+      </c>
       <c r="P41" s="10"/>
       <c r="Q41" s="8">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R41" s="9"/>
       <c r="S41" s="10"/>
@@ -1963,12 +1984,12 @@
         <v>2</v>
       </c>
       <c r="L44" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P44" s="10"/>
       <c r="Q44" s="8">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R44" s="9"/>
       <c r="S44" s="10"/>
@@ -2001,10 +2022,13 @@
       <c r="K45" s="3">
         <v>1</v>
       </c>
+      <c r="L45" s="3">
+        <v>1</v>
+      </c>
       <c r="P45" s="10"/>
       <c r="Q45" s="8">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R45" s="9"/>
       <c r="S45" s="10"/>
@@ -2033,12 +2057,12 @@
         <v>1</v>
       </c>
       <c r="L46" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P46" s="10"/>
       <c r="Q46" s="8">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R46" s="9"/>
       <c r="S46" s="10"/>
@@ -2080,12 +2104,12 @@
         <v>1</v>
       </c>
       <c r="L48" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P48" s="10"/>
       <c r="Q48" s="8">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R48" s="9"/>
       <c r="S48" s="10"/>
@@ -2114,12 +2138,12 @@
         <v>2</v>
       </c>
       <c r="L49" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P49" s="10"/>
       <c r="Q49" s="8">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R49" s="9"/>
       <c r="S49" s="10"/>

</xml_diff>